<commit_message>
chage type declation to follow julia rule
</commit_message>
<xml_diff>
--- a/test/data/append.xlsx
+++ b/test/data/append.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masterplan\.julia\dev\XLSXasJSON\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA8CC62-2787-4795-8F85-ABAF9E1DB0F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6AD4D6-8E98-4C3C-A9C4-3BB967E0AB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,19 +49,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/a/c/1()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/a/c/2()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>aaa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/a/c/2::Vector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/a/c/1::Vector</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D2F80-843F-4BB0-8882-0BEFADD8C837}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -433,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD10D32-8764-4F72-84CF-E7249B4624F6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -473,19 +473,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>